<commit_message>
updating timesheet and adding code from colab to github
</commit_message>
<xml_diff>
--- a/data/raw/Results.xlsx
+++ b/data/raw/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\4th Year\Project\Level-4-Project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519C571F-52FA-46DB-BF94-33C82116B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F83169-3F0D-4474-90D5-579F8BDA063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9 Layer relu with dropout" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="218">
   <si>
     <t>NN(</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>Avg Accuracy</t>
+  </si>
+  <si>
+    <t>in&gt;2100&gt;out</t>
   </si>
 </sst>
 </file>
@@ -824,9 +827,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -841,6 +841,9 @@
     </xf>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5390,6 +5393,56 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7124</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>301596</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BDC7FC9-6C45-5B7F-3392-84336D5C9BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5537974" y="6750050"/>
+          <a:ext cx="1780372" cy="1492250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10489,13 +10542,13 @@
       <c r="C52">
         <v>3.9</v>
       </c>
-      <c r="O52" s="6" t="s">
+      <c r="O52" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="6"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53">
@@ -10507,11 +10560,11 @@
       <c r="C53">
         <v>1.7</v>
       </c>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="6"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54">
@@ -11352,13 +11405,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F6CCC4-3A9C-43D6-AA7B-A2B35C224CFF}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11399,25 +11452,25 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>209</v>
       </c>
       <c r="H3" s="5"/>
@@ -11431,25 +11484,25 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.49</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>0.63</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.46</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>0.51</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>0.49</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <f>(B4+C4+D4+E4+F4)/5</f>
         <v>0.51600000000000001</v>
       </c>
@@ -11464,45 +11517,45 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>0.46200000000000002</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.56399999999999995</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.38300000000000001</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.47399999999999998</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.48799999999999999</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f>(B5+C5+D5+E5+F5)/5</f>
         <v>0.47420000000000001</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>0</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>1</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>2</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>3</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>4</v>
       </c>
       <c r="O5" s="5"/>
@@ -11517,52 +11570,52 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <f>G4</f>
         <v>0.51600000000000001</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <f>G8</f>
         <v>0.44000000000000006</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <f>G12</f>
         <v>0.54399999999999993</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <f>G16</f>
         <v>0.55400000000000005</v>
       </c>
-      <c r="N6" s="10">
-        <f>G21</f>
+      <c r="N6" s="9">
+        <f>G20</f>
         <v>0.59000000000000008</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>209</v>
       </c>
       <c r="H7" s="5"/>
@@ -11576,25 +11629,25 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>0.44</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.4</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.49</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>0.48</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>0.39</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <f>(B8+C8+D8+E8+F8)/5</f>
         <v>0.44000000000000006</v>
       </c>
@@ -11609,25 +11662,25 @@
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>0.377</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.379</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>0.46</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>0.48199999999999998</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>0.34100000000000003</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f>(B9+C9+D9+E9+F9)/5</f>
         <v>0.40780000000000005</v>
       </c>
@@ -11660,25 +11713,25 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>4</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>209</v>
       </c>
       <c r="H11" s="5"/>
@@ -11692,25 +11745,25 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>0.63</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>0.48</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>0.59</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>0.53</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>0.49</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <f>(B12+C12+D12+E12+F12)/5</f>
         <v>0.54399999999999993</v>
       </c>
@@ -11725,25 +11778,25 @@
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0.628</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0.44700000000000001</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>0.52900000000000003</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>0.41399999999999998</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f>(B13+C13+D13+E13+F13)/5</f>
         <v>0.51959999999999995</v>
       </c>
@@ -11776,25 +11829,25 @@
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>2</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>3</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>5</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>209</v>
       </c>
       <c r="H15" s="5"/>
@@ -11808,25 +11861,25 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>0.52</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>0.61</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.49</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>0.61</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>0.54</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f>(B16+C16+D16+E16+F16)/5</f>
         <v>0.55400000000000005</v>
       </c>
@@ -11841,25 +11894,25 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>0.51200000000000001</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0.60199999999999998</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>0.44900000000000001</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>0.56699999999999995</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>0.53100000000000003</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <f>(B17+C17+D17+E17+F17)/5</f>
         <v>0.53220000000000001</v>
       </c>
@@ -11892,13 +11945,27 @@
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -11910,26 +11977,27 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>214</v>
+      <c r="A20" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="B20" s="7">
-        <v>1</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C20" s="7">
-        <v>2</v>
+        <v>0.63</v>
       </c>
       <c r="D20" s="7">
-        <v>3</v>
+        <v>0.54</v>
       </c>
       <c r="E20" s="7">
-        <v>4</v>
+        <v>0.71</v>
       </c>
       <c r="F20" s="7">
-        <v>5</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>209</v>
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="7">
+        <f>(B20+C20+D20+E20+F20)/5</f>
+        <v>0.59000000000000008</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -11942,27 +12010,27 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="8">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C21" s="8">
-        <v>0.63</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0.54</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0.71</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="8">
+      <c r="A21" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.627</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="G21" s="6">
         <f>(B21+C21+D21+E21+F21)/5</f>
-        <v>0.59000000000000008</v>
+        <v>0.58140000000000003</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -11975,28 +12043,6 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B22" s="7">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.627</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="G22" s="7">
-        <f>(B22+C22+D22+E22+F22)/5</f>
-        <v>0.58140000000000003</v>
-      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -12260,12 +12306,24 @@
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="A37" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4</v>
+      </c>
+      <c r="F37" s="5">
+        <v>5</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -12278,7 +12336,9 @@
       <c r="P37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A38" s="5"/>
+      <c r="A38" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>

</xml_diff>